<commit_message>
change micro benchmark graph and better explain.
</commit_message>
<xml_diff>
--- a/draw/perf_data.xlsx
+++ b/draw/perf_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="28035" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="28035" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FW=1" sheetId="1" r:id="rId1"/>
@@ -353,11 +353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="38196352"/>
-        <c:axId val="38197888"/>
+        <c:axId val="109464192"/>
+        <c:axId val="109474176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38196352"/>
+        <c:axId val="109464192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,7 +366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38197888"/>
+        <c:crossAx val="109474176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -374,7 +374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38197888"/>
+        <c:axId val="109474176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -385,14 +385,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38196352"/>
+        <c:crossAx val="109464192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -421,6 +420,26 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Vector of i2</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -599,20 +618,20 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103094528"/>
-        <c:axId val="103100416"/>
+        <c:axId val="111639936"/>
+        <c:axId val="111645824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103094528"/>
+        <c:axId val="111639936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103100416"/>
+        <c:crossAx val="111645824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103100416"/>
+        <c:axId val="111645824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,10 +647,10 @@
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103094528"/>
+        <c:crossAx val="111639936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -667,6 +686,26 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Vector of i4</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -845,20 +884,20 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103089664"/>
-        <c:axId val="103091200"/>
+        <c:axId val="111656320"/>
+        <c:axId val="111752320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103089664"/>
+        <c:axId val="111656320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103091200"/>
+        <c:crossAx val="111752320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -866,7 +905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103091200"/>
+        <c:axId val="111752320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,10 +913,10 @@
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103089664"/>
+        <c:crossAx val="111656320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -913,6 +952,26 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Vector of i4</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1091,20 +1150,20 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="129609728"/>
-        <c:axId val="129611264"/>
+        <c:axId val="111781376"/>
+        <c:axId val="111782912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129609728"/>
+        <c:axId val="111781376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129611264"/>
+        <c:crossAx val="111782912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1112,7 +1171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129611264"/>
+        <c:axId val="111782912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,10 +1179,10 @@
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129609728"/>
+        <c:crossAx val="111781376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1337,11 +1396,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41677952"/>
-        <c:axId val="41679488"/>
+        <c:axId val="109503232"/>
+        <c:axId val="109504768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41677952"/>
+        <c:axId val="109503232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41679488"/>
+        <c:crossAx val="109504768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1358,7 +1417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41679488"/>
+        <c:axId val="109504768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1370,14 +1429,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41677952"/>
+        <c:crossAx val="109503232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1584,11 +1642,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="51951488"/>
-        <c:axId val="51953024"/>
+        <c:axId val="109566976"/>
+        <c:axId val="111293184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51951488"/>
+        <c:axId val="109566976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,7 +1655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51953024"/>
+        <c:crossAx val="111293184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1605,7 +1663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51953024"/>
+        <c:axId val="111293184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1617,7 +1675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51951488"/>
+        <c:crossAx val="109566976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1831,11 +1889,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="54158080"/>
-        <c:axId val="54159616"/>
+        <c:axId val="111309952"/>
+        <c:axId val="111311488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54158080"/>
+        <c:axId val="111309952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,7 +1902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54159616"/>
+        <c:crossAx val="111311488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1852,7 +1910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54159616"/>
+        <c:axId val="111311488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1863,7 +1921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54158080"/>
+        <c:crossAx val="111309952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2077,11 +2135,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="54517120"/>
-        <c:axId val="54523008"/>
+        <c:axId val="110040192"/>
+        <c:axId val="110041728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54517120"/>
+        <c:axId val="110040192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,7 +2148,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54523008"/>
+        <c:crossAx val="110041728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2098,7 +2156,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54523008"/>
+        <c:axId val="110041728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2109,7 +2167,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54517120"/>
+        <c:crossAx val="110040192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2323,11 +2381,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="66377984"/>
-        <c:axId val="66383872"/>
+        <c:axId val="110067072"/>
+        <c:axId val="110077056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66377984"/>
+        <c:axId val="110067072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2336,7 +2394,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66383872"/>
+        <c:crossAx val="110077056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2344,7 +2402,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66383872"/>
+        <c:axId val="110077056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2355,7 +2413,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66377984"/>
+        <c:crossAx val="110067072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2391,6 +2449,26 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Vector of i1</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2569,20 +2647,20 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102912768"/>
-        <c:axId val="102914304"/>
+        <c:axId val="110102016"/>
+        <c:axId val="110103552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102912768"/>
+        <c:axId val="110102016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102914304"/>
+        <c:crossAx val="110103552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2590,7 +2668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102914304"/>
+        <c:axId val="110103552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2598,10 +2676,10 @@
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102912768"/>
+        <c:crossAx val="110102016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2637,6 +2715,26 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Vector of i1</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2815,20 +2913,20 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102947840"/>
-        <c:axId val="102953728"/>
+        <c:axId val="110132608"/>
+        <c:axId val="110142592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102947840"/>
+        <c:axId val="110132608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102953728"/>
+        <c:crossAx val="110142592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2836,7 +2934,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102953728"/>
+        <c:axId val="110142592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2845,10 +2943,10 @@
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102947840"/>
+        <c:crossAx val="110132608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2884,6 +2982,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Vector</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> of i2</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -3062,20 +3184,20 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102895616"/>
-        <c:axId val="102897152"/>
+        <c:axId val="111617536"/>
+        <c:axId val="111619072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102895616"/>
+        <c:axId val="111617536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102897152"/>
+        <c:crossAx val="111619072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3083,7 +3205,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102897152"/>
+        <c:axId val="111619072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3092,10 +3214,10 @@
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102895616"/>
+        <c:crossAx val="111617536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3316,16 +3438,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>16247</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>10085</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>22410</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3350,14 +3472,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>10086</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3380,16 +3502,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>16248</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>20171</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3413,15 +3535,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>45944</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>154639</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>67234</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3444,16 +3566,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>5042</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142314</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3477,15 +3599,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>44263</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>62191</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>56028</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4652,7 +4774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
@@ -6333,8 +6455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>